<commit_message>
Added Book search method in Library_book_list file.
</commit_message>
<xml_diff>
--- a/MainAssignment/DataFile/Book_details.xlsx
+++ b/MainAssignment/DataFile/Book_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>ISBN</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Hacking</t>
+  </si>
+  <si>
+    <t>umar</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -515,6 +527,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added comman variable class for comman use added barrow book class tp barrow book.
</commit_message>
<xml_diff>
--- a/MainAssignment/DataFile/Book_details.xlsx
+++ b/MainAssignment/DataFile/Book_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumarkhan\eclipse-workspace\PIPAssignment\MainAssignment\DataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CF3CD-8081-41AA-B2B2-37DAD7DDAFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504C8524-7F95-4268-858B-806121378DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="2260" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>ISBN</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>1234567890</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
 </sst>
 </file>
@@ -99,10 +96,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -489,11 +492,11 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="E2" t="n">
+        <v>19.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -510,7 +513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -527,7 +530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -540,11 +543,12 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
+      <c r="E5" t="n">
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>